<commit_message>
Add announcement of seminar on Registry studies and HTA
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\GIT\Service\BBS\webpage\home\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -43,6 +43,15 @@
   </si>
   <si>
     <t>29.03.2022</t>
+  </si>
+  <si>
+    <t>Registry studies and health technology assessment (HTA)</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdDpXO5CGgQPrcFj4oz_xWUUOGnGHNU2YkBHjmFXwayqX8BZQ/viewform</t>
+  </si>
+  <si>
+    <t>23.06.2022</t>
   </si>
 </sst>
 </file>
@@ -515,23 +524,32 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>

</xml_diff>

<commit_message>
Added recording, slidedeck of graphical approaches to multiple test problems seminar
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -34,15 +34,6 @@
   </si>
   <si>
     <t>Seminar</t>
-  </si>
-  <si>
-    <t>Graphical approaches to multiple test problems</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/forms/u/1/d/e/1FAIpQLSdC0ei3-k_FNzrFfFtoM4gDXIJJ6BwsvmANLQPlow1XBC-QOA/viewform</t>
-  </si>
-  <si>
-    <t>29.03.2022</t>
   </si>
   <si>
     <t>Registry studies and health technology assessment (HTA)</t>
@@ -497,7 +488,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -525,31 +516,23 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D3" s="11" t="s">
         <v>6</v>
       </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="7"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="1"/>
+      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>

</xml_diff>

<commit_message>
Added announcement of spring seminar "Transforming drug development"
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -44,6 +44,15 @@
   <si>
     <t>23.06.2022</t>
   </si>
+  <si>
+    <t>24.05.2022</t>
+  </si>
+  <si>
+    <t>Transforming drug development</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSfaEQs76ke6olIvtMq88ryPvW3nlW1qd4_1GC0O9w42IJ2mPA/viewform</t>
+  </si>
 </sst>
 </file>
 
@@ -52,7 +61,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -68,12 +77,6 @@
       <sz val="11"/>
       <name val="Arial"/>
       <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
     </font>
     <font>
       <sz val="11"/>
@@ -99,11 +102,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -111,7 +113,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -120,13 +122,13 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -135,12 +137,8 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -488,7 +486,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3:XFD3"/>
+      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -516,23 +514,31 @@
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="C2" s="6" t="s">
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A3" s="7"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="11"/>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="7"/>

</xml_diff>

<commit_message>
Added 1st announcement Next Generation Networking Seminar
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -43,6 +43,12 @@
   </si>
   <si>
     <t>Joint EFSPI &amp; BBS virtual event: Addressing intercurrent events - Treatment policy and hypothetical strategies</t>
+  </si>
+  <si>
+    <t>Next Generation Networking Seminar</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/1RiiijFtDyd6PaZCZ7Xn9rBpboxofP9ccBQ6oa1mhm_s/viewform?ts=63525f94&amp;edit_requested=true</t>
   </si>
 </sst>
 </file>
@@ -171,7 +177,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -199,7 +205,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>16</xdr:row>
+      <xdr:row>17</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -493,11 +499,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E941"/>
+  <dimension ref="A1:E942"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -526,30 +532,35 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="11" t="str">
+    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.35">
+      <c r="A2" s="13" t="str">
+        <f>"30.11.2022"</f>
+        <v>30.11.2022</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="11" t="str">
         <f>"08.12.2022 &amp; 15.12.2022"</f>
         <v>08.12.2022 &amp; 15.12.2022</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B3" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C3" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="14" t="s">
+      <c r="D3" s="14" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="13"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="7"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
@@ -582,7 +593,7 @@
       <c r="C10" s="1"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="2"/>
+      <c r="A11" s="7"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
     </row>
@@ -652,14 +663,14 @@
       <c r="C24" s="1"/>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A25" s="9"/>
+      <c r="A25" s="2"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="9"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="1"/>
+      <c r="C26" s="1"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="9"/>
@@ -708,8 +719,8 @@
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A36" s="9"/>
-      <c r="B36" s="9"/>
-      <c r="C36" s="9"/>
+      <c r="B36" s="4"/>
+      <c r="C36" s="4"/>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="9"/>
@@ -728,13 +739,13 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="9"/>
-      <c r="B40" s="3"/>
-      <c r="C40" s="3"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="9"/>
-      <c r="B41" s="9"/>
-      <c r="C41" s="9"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="9"/>
@@ -773,8 +784,8 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A49" s="9"/>
-      <c r="B49" s="4"/>
-      <c r="C49" s="4"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="9"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A50" s="9"/>
@@ -1342,9 +1353,9 @@
       <c r="C162" s="4"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A163" s="10"/>
-      <c r="B163" s="5"/>
-      <c r="C163" s="5"/>
+      <c r="A163" s="9"/>
+      <c r="B163" s="4"/>
+      <c r="C163" s="4"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A164" s="10"/>
@@ -5236,9 +5247,14 @@
       <c r="B941" s="5"/>
       <c r="C941" s="5"/>
     </row>
+    <row r="942" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A942" s="10"/>
+      <c r="B942" s="5"/>
+      <c r="C942" s="5"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="D3" r:id="rId1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="portrait" r:id="rId2"/>

</xml_diff>

<commit_message>
Added 1st announcement of Good Software Engineering Practice for R Packages
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>date</t>
   </si>
@@ -49,6 +49,15 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/1RiiijFtDyd6PaZCZ7Xn9rBpboxofP9ccBQ6oa1mhm_s/viewform?ts=63525f94&amp;edit_requested=true</t>
+  </si>
+  <si>
+    <t>Good Software Engineering Practice for R Packages</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/1YyZx7ap-QU5gO5RsOziH0jNm4naIBudj0d739jt1Q7Y/viewform?edit_requested=true</t>
   </si>
 </sst>
 </file>
@@ -503,7 +512,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -562,6 +571,21 @@
         <v>6</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="8" t="str">
+        <f>"10.02.2023"</f>
+        <v>10.02.2023</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="7"/>
       <c r="B5" s="1"/>

</xml_diff>

<commit_message>
corrected registration link (v2)
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -57,7 +57,7 @@
     <t>Training</t>
   </si>
   <si>
-    <t>https://docs.google.com/forms/d/1YyZx7ap-QU5gO5RsOziH0jNm4naIBudj0d739jt1Q7Y/viewform?edit_requested=true</t>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdFycbT9dHO-oOyYLUqkKJjM6j5hcL6dQ4uVKC5y8b9RastsA/viewform</t>
   </si>
 </sst>
 </file>
@@ -510,9 +510,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E942"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -582,7 +582,7 @@
       <c r="C4" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="6" t="s">
+      <c r="D4" s="14" t="s">
         <v>12</v>
       </c>
     </row>
@@ -5279,9 +5279,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D3" r:id="rId1"/>
+    <hyperlink ref="D4" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Agenda and registration link for Next Generation event on soft-skills, professional development, and networking
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,25 +1,39 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B94F4E8-A4BD-488F-9B6B-0E2C756677F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="27680" windowHeight="13190"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -65,11 +79,14 @@
   <si>
     <t>Next Generation event on soft-skills, professional development, and networking</t>
   </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSfm0RWYfJ85hdc_ZyRjOMcVYiJ3IOqVepOCZ9d7KU_aixyumA/viewform</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
@@ -175,7 +192,13 @@
     <xdr:ext cx="9525" cy="9525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="image1.gif" descr="https://ssl.gstatic.com/ui/v1/icons/mail/images/cleardot.gif"/>
+        <xdr:cNvPr id="2" name="image1.gif" descr="https://ssl.gstatic.com/ui/v1/icons/mail/images/cleardot.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000002000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -203,7 +226,13 @@
     <xdr:ext cx="9525" cy="9525"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="image1.gif" descr="https://ssl.gstatic.com/ui/v1/icons/mail/images/cleardot.gif"/>
+        <xdr:cNvPr id="3" name="image1.gif" descr="https://ssl.gstatic.com/ui/v1/icons/mail/images/cleardot.gif">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -490,12 +519,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E939"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -554,6 +583,9 @@
       <c r="C3" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>15</v>
+      </c>
     </row>
     <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="str">

</xml_diff>

<commit_message>
Uploaded agenda and registration link for workshop Estimands in Early Development (ED) across Therapeutic Areas
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{823B2D2A-CFA0-41A1-A95B-34C5EE344EEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E227C1C-9DAF-424D-8F85-742CFEF6E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2730" yWindow="1100" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -69,6 +69,15 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/e/1FAIpQLSfm0RWYfJ85hdc_ZyRjOMcVYiJ3IOqVepOCZ9d7KU_aixyumA/viewform</t>
+  </si>
+  <si>
+    <t>Estimands in Early Development (ED) across Therapeutic Areas</t>
+  </si>
+  <si>
+    <t>Workshop</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/1W5vB2AxmrcGLXAz3GWUwfndYgi72D1mGJ6bclbA9m60/viewform?ts=646b293d&amp;edit_requested=true</t>
   </si>
 </sst>
 </file>
@@ -510,9 +519,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E938"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -575,10 +584,20 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="str">
+        <f>"16.10.2023"</f>
+        <v>16.10.2023</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>

</xml_diff>

<commit_message>
Uploaded agenda and registration link for webinar Pre-approval and Post-approval Challenges in the Clinical Development and Reimbursement of CAR-T Cell Therapies
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E227C1C-9DAF-424D-8F85-742CFEF6E29C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98A50A9E-E164-43C4-8678-222FB892C245}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2730" yWindow="1100" windowWidth="14400" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -71,13 +71,22 @@
     <t>https://docs.google.com/forms/d/e/1FAIpQLSfm0RWYfJ85hdc_ZyRjOMcVYiJ3IOqVepOCZ9d7KU_aixyumA/viewform</t>
   </si>
   <si>
-    <t>Estimands in Early Development (ED) across Therapeutic Areas</t>
-  </si>
-  <si>
     <t>Workshop</t>
   </si>
   <si>
     <t>https://docs.google.com/forms/d/1W5vB2AxmrcGLXAz3GWUwfndYgi72D1mGJ6bclbA9m60/viewform?ts=646b293d&amp;edit_requested=true</t>
+  </si>
+  <si>
+    <t>CAR-T Cell Therapies</t>
+  </si>
+  <si>
+    <t>Pre-approval and Post-approval Challenges in the Clinical Development and Reimbursement of CAR-T Cell Therapies</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/17xP-k8lVxfUTwdhQrSNR_tg391r5WM5Cc6CXElYH_Ic/viewform?edit_requested=true</t>
+  </si>
+  <si>
+    <t>2 days, 04.-05.10.2023</t>
   </si>
 </sst>
 </file>
@@ -183,7 +192,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -217,7 +226,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>13</xdr:row>
+      <xdr:row>14</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -517,11 +526,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E938"/>
+  <dimension ref="A1:E939"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -584,25 +593,38 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="str">
+        <f>"04.10.2023"</f>
+        <v>04.10.2023</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="6" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="str">
         <f>"16.10.2023"</f>
         <v>16.10.2023</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="D5" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="6" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="2"/>
@@ -685,14 +707,14 @@
       <c r="C21" s="1"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A22" s="8"/>
+      <c r="A22" s="2"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A23" s="8"/>
-      <c r="B23" s="4"/>
-      <c r="C23" s="4"/>
+      <c r="B23" s="1"/>
+      <c r="C23" s="1"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A24" s="8"/>
@@ -741,8 +763,8 @@
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A33" s="8"/>
-      <c r="B33" s="8"/>
-      <c r="C33" s="8"/>
+      <c r="B33" s="4"/>
+      <c r="C33" s="4"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A34" s="8"/>
@@ -761,13 +783,13 @@
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A37" s="8"/>
-      <c r="B37" s="3"/>
-      <c r="C37" s="3"/>
+      <c r="B37" s="8"/>
+      <c r="C37" s="8"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A38" s="8"/>
-      <c r="B38" s="8"/>
-      <c r="C38" s="8"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
@@ -806,8 +828,8 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="8"/>
-      <c r="B46" s="4"/>
-      <c r="C46" s="4"/>
+      <c r="B46" s="8"/>
+      <c r="C46" s="8"/>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="8"/>
@@ -1375,9 +1397,9 @@
       <c r="C159" s="4"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A160" s="9"/>
-      <c r="B160" s="5"/>
-      <c r="C160" s="5"/>
+      <c r="A160" s="8"/>
+      <c r="B160" s="4"/>
+      <c r="C160" s="4"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A161" s="9"/>
@@ -5268,6 +5290,11 @@
       <c r="A938" s="9"/>
       <c r="B938" s="5"/>
       <c r="C938" s="5"/>
+    </row>
+    <row r="939" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A939" s="9"/>
+      <c r="B939" s="5"/>
+      <c r="C939" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
Added registration link for Next Generation BBS Training Day on Dec 6th, 2023
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B65572EB-4102-4392-8617-195C751842A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94AC5705-6A90-427C-AA14-F21A1A4E4D9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -66,6 +66,9 @@
   </si>
   <si>
     <t>Training</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSdNHRAhz04hFxlFNf-4yk4Mp7fLafW9o35ahL5uZWgO-kX1PQ/viewform?usp=sf_link</t>
   </si>
 </sst>
 </file>
@@ -518,9 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E935"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -579,6 +582,9 @@
       <c r="C3" s="1" t="s">
         <v>10</v>
       </c>
+      <c r="D3" s="10" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
@@ -5243,9 +5249,10 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D3" r:id="rId2" xr:uid="{FDD9243E-6558-4D0E-84B1-18A4D70177AC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
+  <drawing r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uploaded slides for Next Generation BBS Training Day on Dec 6th, 2023
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C48D79A4-A3AE-4323-8DC3-FFFBBCC63E56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06A47CB4-2EED-4D10-9A97-621BC364EF60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -54,9 +54,6 @@
   </si>
   <si>
     <t>Training</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/forms/d/e/1FAIpQLSdNHRAhz04hFxlFNf-4yk4Mp7fLafW9o35ahL5uZWgO-kX1PQ/viewform?usp=sf_link</t>
   </si>
 </sst>
 </file>
@@ -511,7 +508,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -552,9 +549,7 @@
       <c r="C2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="10" t="s">
-        <v>7</v>
-      </c>
+      <c r="D2" s="10"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="2"/>
@@ -5217,11 +5212,8 @@
       <c r="C934" s="5"/>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{FDD9243E-6558-4D0E-84B1-18A4D70177AC}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
-  <drawing r:id="rId3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
uploaded first announcement for Reproducibility in biomedical research (Apr 12th)
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C559873E-ECB5-4536-9060-02506CA37E7C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FDD97-A767-420D-86F1-83EC680A172A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>date</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>February 12th &amp; 13th, 2024</t>
+  </si>
+  <si>
+    <t>Reproducibility in biomedical research</t>
+  </si>
+  <si>
+    <t>Seminar</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSfhQ2QXOS6pUtW6tVJmTWCpJ1viDrsRciQaC7Fa4Rn8A11Bzg/viewform</t>
   </si>
 </sst>
 </file>
@@ -512,9 +521,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -563,9 +572,19 @@
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+      <c r="A3" s="2" t="str">
+        <f>"12.04.2024"</f>
+        <v>12.04.2024</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>

</xml_diff>

<commit_message>
uploaded first announcement for Next Generation event on visualization
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{193FDD97-A767-420D-86F1-83EC680A172A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1ABAC9-02C4-483A-B542-AFE500F0A683}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>date</t>
   </si>
@@ -69,6 +69,9 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/e/1FAIpQLSfhQ2QXOS6pUtW6tVJmTWCpJ1viDrsRciQaC7Fa4Rn8A11Bzg/viewform</t>
+  </si>
+  <si>
+    <t>Next Generation event on visualization</t>
   </si>
 </sst>
 </file>
@@ -521,9 +524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E934"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
+      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -587,9 +590,16 @@
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+      <c r="A4" s="2" t="str">
+        <f>"17.04.2024"</f>
+        <v>17.04.2024</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>

</xml_diff>

<commit_message>
updated first announcement BBS NextGen event on Mar 4 w/ registration link
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65765DEB-3A39-49CD-9E19-CE10C708AEE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55ED896-F85F-431C-84A4-6CB48E30D411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -60,6 +60,12 @@
   </si>
   <si>
     <t>Next Generation event on visualization</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSeihutW5e1eUk950jLWmTtZGe9xD099mjazpOuueLLhHczpHg/closedform</t>
+  </si>
+  <si>
+    <t>Registration opens on Monday, Mar 4th.</t>
   </si>
 </sst>
 </file>
@@ -501,9 +507,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E933"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -559,6 +565,12 @@
       <c r="C3" s="1" t="s">
         <v>6</v>
       </c>
+      <c r="D3" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>

</xml_diff>

<commit_message>
upload first announcement and agenda for Essentials of Medical Data Sharing and Privacy - Maximize the use of data (May 16th, 2024)
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F55ED896-F85F-431C-84A4-6CB48E30D411}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6EDBC8D-5F08-4FE8-9E22-827FEDACB03D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>date</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Registration opens on Monday, Mar 4th.</t>
+  </si>
+  <si>
+    <t>Essentials of Medical Data Sharing and Privacy – Maximize the use of data</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLScginwB-LRjoMPtq9rVpYPF7KLkhLg1DCUCirWNj0Qdx0muug/viewform</t>
   </si>
 </sst>
 </file>
@@ -509,7 +515,7 @@
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomLeft" activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -572,10 +578,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="2"/>
-      <c r="B4" s="1"/>
-      <c r="C4" s="1"/>
+    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="str">
+        <f>"16.05.2024"</f>
+        <v>16.05.2024</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4" s="6" t="s">
+        <v>12</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>

</xml_diff>

<commit_message>
move NextGen event on visualizations from Apr 17th, 2024 from "upcoming" to "past"
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29E3B73E-756F-496E-BCC9-720CD18F14F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A9B7429-54A8-4102-9AC9-E3CB7936664E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1340" yWindow="1880" windowWidth="14380" windowHeight="7360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -50,12 +50,6 @@
   </si>
   <si>
     <t>Seminar</t>
-  </si>
-  <si>
-    <t>Next Generation event on visualization</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/forms/d/e/1FAIpQLSeihutW5e1eUk950jLWmTtZGe9xD099mjazpOuueLLhHczpHg/closedform</t>
   </si>
   <si>
     <t>Essentials of Medical Data Sharing and Privacy – Maximize the use of data</t>
@@ -173,7 +167,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -207,7 +201,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>7</xdr:row>
+      <xdr:row>6</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -507,11 +501,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E932"/>
+  <dimension ref="A1:E931"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -541,10 +535,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="str">
-        <f>"17.04.2024"</f>
-        <v>17.04.2024</v>
+        <f>"16.05.2024"</f>
+        <v>16.05.2024</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
@@ -558,8 +552,8 @@
     </row>
     <row r="3" spans="1:5" ht="28" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="str">
-        <f>"16.05.2024"</f>
-        <v>16.05.2024</v>
+        <f>"29.08.2024"</f>
+        <v>29.08.2024</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>8</v>
@@ -571,20 +565,10 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="28" x14ac:dyDescent="0.35">
-      <c r="A4" s="2" t="str">
-        <f>"29.08.2024"</f>
-        <v>29.08.2024</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" s="6" t="s">
-        <v>11</v>
-      </c>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="2"/>
+      <c r="B4" s="1"/>
+      <c r="C4" s="1"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="2"/>
@@ -637,14 +621,14 @@
       <c r="C14" s="1"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="2"/>
+      <c r="A15" s="8"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="8"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
+      <c r="B16" s="4"/>
+      <c r="C16" s="4"/>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A17" s="8"/>
@@ -693,8 +677,8 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A26" s="8"/>
-      <c r="B26" s="4"/>
-      <c r="C26" s="4"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A27" s="8"/>
@@ -713,13 +697,13 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A30" s="8"/>
-      <c r="B30" s="8"/>
-      <c r="C30" s="8"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A31" s="8"/>
-      <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="B31" s="8"/>
+      <c r="C31" s="8"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A32" s="8"/>
@@ -758,8 +742,8 @@
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="8"/>
-      <c r="B39" s="8"/>
-      <c r="C39" s="8"/>
+      <c r="B39" s="4"/>
+      <c r="C39" s="4"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="8"/>
@@ -1327,9 +1311,9 @@
       <c r="C152" s="4"/>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A153" s="8"/>
-      <c r="B153" s="4"/>
-      <c r="C153" s="4"/>
+      <c r="A153" s="9"/>
+      <c r="B153" s="5"/>
+      <c r="C153" s="5"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A154" s="9"/>
@@ -5220,11 +5204,6 @@
       <c r="A931" s="9"/>
       <c r="B931" s="5"/>
       <c r="C931" s="5"/>
-    </row>
-    <row r="932" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A932" s="9"/>
-      <c r="B932" s="5"/>
-      <c r="C932" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>

</xml_diff>

<commit_message>
uploaded first announcement for NextGen event Thriving Careers: Navigating Bias, Reinventing Yourself, and Essential Skills for Employability
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27726"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F8BB54E-28E3-401F-96D2-D29D9E6D5B4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87472379-E5A3-40FD-AB55-E8581F86EE08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
   <si>
     <t>date</t>
   </si>
@@ -57,6 +57,12 @@
   <si>
     <t>https://docs.google.com/forms/d/e/1FAIpQLSe5dfKHdN6JdKAFsE8Zw1CUs7soHzgrZb9-YCLGa4PRcxWoBQ/viewform</t>
   </si>
+  <si>
+    <t>Next Generation event on Thriving Careers: Navigating Bias, Reinventing Yourself, and Essential Skills for Employability</t>
+  </si>
+  <si>
+    <t>Registration is scheduled to open at the end of August 2024.</t>
+  </si>
 </sst>
 </file>
 
@@ -65,7 +71,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd&quot;.&quot;mm&quot;.&quot;yyyy"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -88,6 +94,11 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF544F4F"/>
+      <name val="Roche Sans Light"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -109,7 +120,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -138,6 +149,7 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,9 +509,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E930"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="68" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -544,10 +556,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A3" s="2"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
+    <row r="3" spans="1:5" ht="42" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="str">
+        <f>"20.09.2024"</f>
+        <v>20.09.2024</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="10"/>
+      <c r="E3" s="6" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>

</xml_diff>

<commit_message>
upload 1st announcement of Patient-Focused Drug Development: The Role of Patient Preference Studies
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GIT\Service\BBS\webpage\home\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB83A1AE-736B-426C-B6F6-B3AC3CEAFA42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4CAD8E9-718A-41F0-8019-7D45A21B88E7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="15">
   <si>
     <t>date</t>
   </si>
@@ -68,6 +68,15 @@
   </si>
   <si>
     <t>AI in Clinical Research and Drug Development and BBS General Assembly</t>
+  </si>
+  <si>
+    <t>Patient-Focused Drug Development: The Role of Patient Preference Studies</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSfTzB87PDyKV4wxd0j9c8LkAQlwfWDQvLeAGjlr9mGDBNk3rQ/viewform</t>
   </si>
 </sst>
 </file>
@@ -515,9 +524,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E930"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="122" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
+      <selection pane="bottomLeft" activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.453125" defaultRowHeight="14.5"/>
@@ -593,10 +602,20 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
-      <c r="A5" s="2"/>
-      <c r="B5" s="1"/>
-      <c r="C5" s="1"/>
+    <row r="5" spans="1:5" ht="28">
+      <c r="A5" s="2" t="str">
+        <f>"22.10.2024"</f>
+        <v>22.10.2024</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2"/>

</xml_diff>

<commit_message>
Add April NextGen lunch
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10315"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10402"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/widmelu1/Documents/git/bbs-basel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A58874DF-D98D-2D46-887B-00FF0E670C96}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51AC834E-F3AA-B84B-97ED-C62498C81ECA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1900" yWindow="1780" windowWidth="27860" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="52340" yWindow="1200" windowWidth="27860" windowHeight="19840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>date</t>
   </si>
@@ -49,22 +49,13 @@
     <t>comment</t>
   </si>
   <si>
-    <t>Seminar</t>
-  </si>
-  <si>
-    <t>BBS Meeting on Covariate adjustment in clinical trials</t>
-  </si>
-  <si>
-    <t>https://docs.google.com/forms/d/e/1FAIpQLSeEge5cqx9Ae6lok_S6kTFH0bAjjJhTVIEcwL6MOffM3QTnbw/viewform</t>
-  </si>
-  <si>
     <t>Networking</t>
   </si>
   <si>
     <t>BBS NextGen Lunch</t>
   </si>
   <si>
-    <t>https://calendarlink.com/event/8NxmZ</t>
+    <t>https://calendarlink.com/event/e2fR0</t>
   </si>
 </sst>
 </file>
@@ -196,7 +187,7 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -230,7 +221,7 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="9525" cy="9525"/>
@@ -534,7 +525,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D4" sqref="D4"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -565,34 +556,21 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="str">
-        <f>"25.03.2025"</f>
-        <v>25.03.2025</v>
+      <c r="A2" s="10" t="str">
+        <f>"24.04.2025"</f>
+        <v>24.04.2025</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="10" t="str">
-        <f>"28.03.2025"</f>
-        <v>28.03.2025</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3" s="14" t="s">
-        <v>10</v>
-      </c>
       <c r="E3" s="11"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
@@ -5212,11 +5190,10 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{8D7C6BEB-722D-4874-B77E-6264F787DC62}"/>
-    <hyperlink ref="D3" r:id="rId2" xr:uid="{7270A489-9841-EF49-BC21-4417FBF858C4}"/>
+    <hyperlink ref="D2" r:id="rId1" xr:uid="{7270A489-9841-EF49-BC21-4417FBF858C4}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
-  <pageSetup orientation="portrait" r:id="rId3"/>
-  <drawing r:id="rId4"/>
+  <pageSetup orientation="portrait" r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Correct date for May BBS Next Gen Lunch
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -167,27 +167,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -199,27 +199,27 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -307,9 +307,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -323,7 +323,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7197840" y="181080"/>
-          <a:ext cx="9000" cy="9000"/>
+          <a:ext cx="8640" cy="8640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -344,9 +344,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9000</xdr:colOff>
+      <xdr:colOff>8640</xdr:colOff>
       <xdr:row>1</xdr:row>
-      <xdr:rowOff>9000</xdr:rowOff>
+      <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -360,7 +360,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="0" y="181080"/>
-          <a:ext cx="9000" cy="9000"/>
+          <a:ext cx="8640" cy="8640"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -557,7 +557,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="122" zoomScaleNormal="122" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D3" activeCellId="0" sqref="D3"/>
+      <selection pane="bottomLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.4453125" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -587,10 +587,10 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="14.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="str">
-        <f aca="false">"24.04.2025"</f>
-        <v>24.04.2025</v>
+        <f aca="false">"23.05.2025"</f>
+        <v>23.05.2025</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>5</v>

</xml_diff>

<commit_message>
added first announcement for BBS Seminar: Causal mediation analysis in clinical research
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69757D3D-D8F5-4364-A8BD-42EF6A5F0338}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD1B6B80-ACFC-4A4E-A22F-2E8148CA22A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3300" yWindow="3720" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3480" yWindow="5412" windowWidth="17280" windowHeight="9960" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>date</t>
   </si>
@@ -85,6 +85,12 @@
   <si>
     <t>Dates: October 14th, 13:00-17:00 and October 15th, 8:30-12:00; Location: Novartis Campus, Basel, Switzerland; Registration is mandatory and will open in August.</t>
   </si>
+  <si>
+    <t>Causal mediation analysis in clinical research</t>
+  </si>
+  <si>
+    <t>https://tally.so/r/mRQ7NJ</t>
+  </si>
 </sst>
 </file>
 
@@ -93,7 +99,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -133,6 +139,13 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -151,10 +164,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -187,8 +201,12 @@
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -541,9 +559,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E926"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -635,9 +653,19 @@
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="3"/>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
+      <c r="A6" s="3" t="str">
+        <f>"30.10.2025"</f>
+        <v>30.10.2025</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="3"/>
@@ -5240,8 +5268,11 @@
       <c r="C926" s="10"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{C08CD0DC-37C8-4175-AA2D-98F427EA6018}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Remove outdated lunch and update EFSPI NextGen Event agenda
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10810"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10824"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/widmelu1/Documents/git/bbs-basel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{790F7732-E145-8A44-8A9F-B2F0FC935539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{48AF1720-FAE4-EE4A-9643-B6E4F47886AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="66140" yWindow="12900" windowWidth="32620" windowHeight="13780" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
   <si>
     <t>date</t>
   </si>
@@ -84,15 +84,6 @@
   </si>
   <si>
     <t>Registration closed</t>
-  </si>
-  <si>
-    <t>BBS NextGen Lunch Special Edition</t>
-  </si>
-  <si>
-    <t>13:00, St Louis Buvette</t>
-  </si>
-  <si>
-    <t>BBS NextGen Lunch ISCB Special Edition</t>
   </si>
 </sst>
 </file>
@@ -147,7 +138,7 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
-      <charset val="1"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -171,7 +162,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -206,9 +197,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -302,13 +290,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -345,13 +333,13 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>0</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
-      <xdr:row>2</xdr:row>
+      <xdr:row>1</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -567,7 +555,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -597,79 +585,64 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A2" s="13" t="str">
-        <f>"28.08.2025"</f>
-        <v>28.08.2025</v>
-      </c>
-      <c r="B2" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C2" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="str">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="str">
         <f>"09.09.2025"</f>
         <v>09.09.2025</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E3" s="11" t="s">
+      <c r="E2" s="11" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="str">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="str">
         <f>"14.10.2025"</f>
         <v>14.10.2025</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="11"/>
-      <c r="E4" s="2" t="s">
+      <c r="D3" s="11"/>
+      <c r="E3" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="30" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="str">
+    <row r="4" spans="1:5" ht="30" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="str">
         <f>"16.10.2025"</f>
         <v>16.10.2025</v>
       </c>
+      <c r="B4" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="str">
+        <f>"30.10.2025"</f>
+        <v>30.10.2025</v>
+      </c>
       <c r="B5" s="4" t="s">
-        <v>9</v>
+        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="str">
-        <f>"30.10.2025"</f>
-        <v>30.10.2025</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D6" s="12" t="s">
+      <c r="D5" s="12" t="s">
         <v>14</v>
       </c>
     </row>
@@ -5275,7 +5248,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D6" r:id="rId1" xr:uid="{C08CD0DC-37C8-4175-AA2D-98F427EA6018}"/>
+    <hyperlink ref="D5" r:id="rId1" xr:uid="{C08CD0DC-37C8-4175-AA2D-98F427EA6018}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
uploaded 1st announcement for Patient Preference Studies: What Do We Know Now? (17 Sep 2025)
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B711832B-8429-48F3-AEB1-3D84BC8E0E71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5D71AC-3612-49D3-8A56-5ED3ED8B4F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>date</t>
   </si>
@@ -91,6 +91,15 @@
   <si>
     <t>https://docs.google.com/forms/d/e/1FAIpQLSdngL6zFUwDodqpVKdHu9oTtVBjUF7iGYkM8yFpzvc4zB_DBw/viewform?usp=send_form</t>
   </si>
+  <si>
+    <t>Patient Preference Studies: What Do We Know Now?</t>
+  </si>
+  <si>
+    <t>BBS – Suisse Romandie Webinar</t>
+  </si>
+  <si>
+    <t>https://docs.google.com/forms/d/e/1FAIpQLSeVdFVpdzFkW7ztYY9C--SDwvhdMFH8LR353oJ9ecD-AsJxPw/viewform</t>
+  </si>
 </sst>
 </file>
 
@@ -99,7 +108,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -146,6 +155,12 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF333333"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -168,7 +183,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -204,6 +219,7 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,11 +573,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E926"/>
+  <dimension ref="A1:E927"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
+      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -608,69 +624,80 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="str">
+        <f>"17.09.2025"</f>
+        <v>17.09.2025</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E3" s="11"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="str">
         <f>"14.10.2025"</f>
         <v>14.10.2025</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B4" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C4" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="11"/>
-      <c r="E3" s="2" t="s">
+      <c r="D4" s="11"/>
+      <c r="E4" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="str">
+    <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="str">
         <f>"16.10.2025"</f>
         <v>16.10.2025</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="B5" s="4" t="s">
         <v>9</v>
-      </c>
-      <c r="C4" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" s="3" t="str">
-        <f>"30.10.2025"</f>
-        <v>30.10.2025</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>13</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A6" s="3" t="str">
+        <f>"30.10.2025"</f>
+        <v>30.10.2025</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="12" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A6" s="1" t="str">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="str">
         <f>"31.10.2025"</f>
         <v>31.10.2025</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B7" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C7" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D7" s="12" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="3"/>
@@ -683,14 +710,14 @@
       <c r="C9" s="4"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A10" s="5"/>
+      <c r="A10" s="3"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
-      <c r="C11" s="6"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A12" s="5"/>
@@ -722,14 +749,14 @@
       <c r="B17" s="6"/>
       <c r="C17" s="6"/>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="7"/>
+      <c r="B18" s="6"/>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5"/>
-      <c r="B19" s="6"/>
+      <c r="B19" s="7"/>
       <c r="C19" s="6"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
@@ -739,8 +766,8 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" s="5"/>
-      <c r="B21" s="5"/>
-      <c r="C21" s="5"/>
+      <c r="B21" s="6"/>
+      <c r="C21" s="6"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" s="5"/>
@@ -759,13 +786,13 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" s="5"/>
-      <c r="B25" s="8"/>
-      <c r="C25" s="8"/>
+      <c r="B25" s="5"/>
+      <c r="C25" s="5"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="5"/>
-      <c r="C26" s="5"/>
+      <c r="B26" s="8"/>
+      <c r="C26" s="8"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
@@ -804,8 +831,8 @@
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" s="5"/>
-      <c r="B34" s="6"/>
-      <c r="C34" s="6"/>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" s="5"/>
@@ -1373,9 +1400,9 @@
       <c r="C147" s="6"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="9"/>
-      <c r="B148" s="10"/>
-      <c r="C148" s="10"/>
+      <c r="A148" s="5"/>
+      <c r="B148" s="6"/>
+      <c r="C148" s="6"/>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A149" s="9"/>
@@ -5267,10 +5294,15 @@
       <c r="B926" s="10"/>
       <c r="C926" s="10"/>
     </row>
+    <row r="927" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A927" s="9"/>
+      <c r="B927" s="10"/>
+      <c r="C927" s="10"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D5" r:id="rId1" xr:uid="{C08CD0DC-37C8-4175-AA2D-98F427EA6018}"/>
-    <hyperlink ref="D6" r:id="rId2" xr:uid="{8AE13CAA-8ABC-4A14-A257-6D73CC5EDE75}"/>
+    <hyperlink ref="D6" r:id="rId1" xr:uid="{C08CD0DC-37C8-4175-AA2D-98F427EA6018}"/>
+    <hyperlink ref="D7" r:id="rId2" xr:uid="{8AE13CAA-8ABC-4A14-A257-6D73CC5EDE75}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>

</xml_diff>

<commit_message>
uploaded 1st announcement for F2F BBS Training: Data Monitoring Committees (DMCs), Oct 14th - 15th, 2025
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC5D71AC-3612-49D3-8A56-5ED3ED8B4F0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D79EAA6-7D1A-4D1A-B182-56A0936B8051}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -68,13 +68,7 @@
     <t>Colloquium in Honor of Hans Ulrich Burger on the Occasion of His Retirement from Roche</t>
   </si>
   <si>
-    <t>F2F course on Data Monitoring Committees (DMCs) for clinical trials and clinical development programs</t>
-  </si>
-  <si>
     <t>BBS Training</t>
-  </si>
-  <si>
-    <t>Dates: October 14th, 13:00-17:00 and October 15th, 8:30-12:00; Location: Novartis Campus, Basel, Switzerland; Registration is mandatory and will open in August.</t>
   </si>
   <si>
     <t>Causal mediation analysis in clinical research</t>
@@ -99,6 +93,12 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/e/1FAIpQLSeVdFVpdzFkW7ztYY9C--SDwvhdMFH8LR353oJ9ecD-AsJxPw/viewform</t>
+  </si>
+  <si>
+    <t>F2F course on Data Monitoring Committees (DMCs)</t>
+  </si>
+  <si>
+    <t>Registration is mandatory. A nominal registration fee of CHF50 will be charged. To register, please email Tobias Muetze (tobias.muetze@novartis.com). Payment details will be shared after registration.</t>
   </si>
 </sst>
 </file>
@@ -575,9 +575,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E927"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -619,7 +619,7 @@
         <v>6</v>
       </c>
       <c r="E2" s="11" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.3">
@@ -628,13 +628,13 @@
         <v>17.09.2025</v>
       </c>
       <c r="B3" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E3" s="11"/>
     </row>
@@ -644,14 +644,14 @@
         <v>14.10.2025</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D4" s="11"/>
       <c r="E4" s="2" t="s">
-        <v>12</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
@@ -675,13 +675,13 @@
         <v>30.10.2025</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.3">
@@ -690,13 +690,13 @@
         <v>31.10.2025</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D7" s="12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Add BBS Workshop on the False Discovery Rate
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10921"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11003"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/widmelu1/Documents/git/bbs-basel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A211D1C-23DA-D44C-A4FD-7E939A06AA6F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53CB76A-4C34-474E-A6B6-EAD40F7B43C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="58660" yWindow="-1260" windowWidth="23260" windowHeight="13900" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="26860" yWindow="8580" windowWidth="60160" windowHeight="31940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
   <si>
     <t>date</t>
   </si>
@@ -90,6 +90,15 @@
   </si>
   <si>
     <t xml:space="preserve">https://calendarlink.com/event/0Uarc </t>
+  </si>
+  <si>
+    <t>BBS Workshop</t>
+  </si>
+  <si>
+    <t>BBS Workshop on the False Discovery Rate</t>
+  </si>
+  <si>
+    <t>https://forms.gle/j1EnwYEkYcRjN67X9</t>
   </si>
 </sst>
 </file>
@@ -162,7 +171,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -200,6 +209,7 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -557,7 +567,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -659,9 +669,19 @@
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A7" s="3"/>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
+      <c r="A7" s="12" t="str">
+        <f>"24.11.2025"</f>
+        <v>24.11.2025</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="3"/>
@@ -5258,10 +5278,11 @@
     <hyperlink ref="D4" r:id="rId1" xr:uid="{C08CD0DC-37C8-4175-AA2D-98F427EA6018}"/>
     <hyperlink ref="D5" r:id="rId2" xr:uid="{8AE13CAA-8ABC-4A14-A257-6D73CC5EDE75}"/>
     <hyperlink ref="D3" r:id="rId3" xr:uid="{43C6464F-F741-324A-9993-990D6C8E50C0}"/>
+    <hyperlink ref="D7" r:id="rId4" xr:uid="{8E307D8A-6F21-3B4F-97D7-C148E439068A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId4"/>
+  <drawing r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Add BBS Suisse Romandie
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/widmelu1/Documents/git/bbs-basel/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F53CB76A-4C34-474E-A6B6-EAD40F7B43C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D894650-EF93-3341-A663-1238A4F32714}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="26860" yWindow="8580" windowWidth="60160" windowHeight="31940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="60160" windowHeight="31940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="upcoming" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="22">
   <si>
     <t>date</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>https://forms.gle/j1EnwYEkYcRjN67X9</t>
+  </si>
+  <si>
+    <t>https://forms.gle/GUppmYMqPVSJ6VBX9</t>
   </si>
 </sst>
 </file>
@@ -567,14 +570,14 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D8" sqref="D8"/>
+      <selection pane="bottomLeft" activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
     <col min="2" max="2" width="70" style="2" customWidth="1"/>
-    <col min="3" max="3" width="20.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="23.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="35.6640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="9.5" style="2" customWidth="1"/>
     <col min="6" max="16384" width="14.5" style="2"/>
@@ -667,6 +670,9 @@
       <c r="C6" s="2" t="s">
         <v>15</v>
       </c>
+      <c r="D6" s="11" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="12" t="str">
@@ -5279,10 +5285,11 @@
     <hyperlink ref="D5" r:id="rId2" xr:uid="{8AE13CAA-8ABC-4A14-A257-6D73CC5EDE75}"/>
     <hyperlink ref="D3" r:id="rId3" xr:uid="{43C6464F-F741-324A-9993-990D6C8E50C0}"/>
     <hyperlink ref="D7" r:id="rId4" xr:uid="{8E307D8A-6F21-3B4F-97D7-C148E439068A}"/>
+    <hyperlink ref="D6" r:id="rId5" xr:uid="{98DB2844-BB1B-144B-8BE3-46ED5AE75040}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
Posted the first announcement and save-the-date for the BBS Training: 'Does This Treatment Cause That Outcome? A Practical Guide to Estimand Thinking.'
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7247812-2448-4DFA-9493-02DB1C6D8457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC5486C1-3E63-4E0E-A498-6F46AEE8D54D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>date</t>
   </si>
@@ -52,6 +52,12 @@
   <si>
     <t>comment</t>
   </si>
+  <si>
+    <t>Does This Treatment Cause That Outcome: A Practical Guide to Estimand Thinking</t>
+  </si>
+  <si>
+    <t>Training</t>
+  </si>
 </sst>
 </file>
 
@@ -60,7 +66,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -94,6 +100,13 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <b/>
+      <sz val="16"/>
+      <color rgb="FF000000"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -115,7 +128,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -147,6 +160,10 @@
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,7 +477,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -490,14 +507,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" s="5"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A2" s="5" t="str">
+        <f>"25.03.2026"</f>
+        <v>25.03.2026</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>5</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A3" s="5"/>
-      <c r="B3" s="6"/>
+      <c r="B3" s="12"/>
       <c r="C3" s="6"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
added registration link for Optimizing Multiple Comparisons in Sequential and Non-Sequential Clinical Trials webinar on Mar 11, 2026 (announcement is pending)
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2353520-95B0-485F-A164-EEA2CBE724C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5D8BB7B6-0A84-4212-8D62-E382CE360CA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/1OiFtrYu6YPpKNzTIqmSs3j-CDwCPOZvNI6u5od-ewAo/viewform?ts=69722637&amp;edit_requested=true</t>
+  </si>
+  <si>
+    <t>Optimizing Multiple Comparisons in Sequential and Non-Sequential Clinical Trials</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>https://forms.gle/UJ9TLAbqHaapnN687</t>
   </si>
 </sst>
 </file>
@@ -270,13 +279,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -488,7 +497,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E918"/>
+  <dimension ref="A1:E919"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
@@ -522,29 +531,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="str">
+    <row r="2" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="str">
+        <f>"11.03.2026"</f>
+        <v>11.03.2026</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="str">
         <f>"25.03.2026"</f>
         <v>25.03.2026</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,14 +591,14 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -589,8 +608,8 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -609,13 +628,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
@@ -654,8 +673,8 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
@@ -1223,9 +1242,9 @@
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="9"/>
-      <c r="B140" s="10"/>
-      <c r="C140" s="10"/>
+      <c r="A140" s="5"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="9"/>
@@ -5117,13 +5136,19 @@
       <c r="B918" s="10"/>
       <c r="C918" s="10"/>
     </row>
+    <row r="919" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A919" s="9"/>
+      <c r="B919" s="10"/>
+      <c r="C919" s="10"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{52F67EFF-01EC-4C1D-ACB7-B5A4E4927918}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{52F67EFF-01EC-4C1D-ACB7-B5A4E4927918}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{DB7641CF-F3CB-4B72-81FA-C26EDCB07C96}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
added first announcement for Optimizing Multiple Comparisons in Sequential and Non-Sequential Clinical Trials (Mar 9th [!] 2026)
</commit_message>
<xml_diff>
--- a/data/upcoming.xlsx
+++ b/data/upcoming.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\schaej17\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{325ABD0D-982D-4C60-AE57-7D7569954810}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F55FEA8-A6FC-45C7-AF29-677F09CD0307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>date</t>
   </si>
@@ -60,6 +60,15 @@
   </si>
   <si>
     <t>https://docs.google.com/forms/d/1OiFtrYu6YPpKNzTIqmSs3j-CDwCPOZvNI6u5od-ewAo/viewform?ts=69722637&amp;edit_requested=true</t>
+  </si>
+  <si>
+    <t>Optimizing Multiple Comparisons in Sequential and Non-Sequential Clinical Trials</t>
+  </si>
+  <si>
+    <t>Webinar</t>
+  </si>
+  <si>
+    <t>https://forms.gle/UJ9TLAbqHaapnN687</t>
   </si>
 </sst>
 </file>
@@ -270,13 +279,13 @@
     <xdr:from>
       <xdr:col>4</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>8640</xdr:colOff>
-      <xdr:row>1</xdr:row>
+      <xdr:row>2</xdr:row>
       <xdr:rowOff>8640</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -488,11 +497,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E918"/>
+  <dimension ref="A1:E919"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="122" zoomScaleNormal="122" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2:XFD2"/>
+      <selection pane="bottomLeft" activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -522,29 +531,39 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
-      <c r="A2" s="5" t="str">
+    <row r="2" spans="1:5" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="str">
+        <f>"09.03.2026"</f>
+        <v>09.03.2026</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A3" s="5" t="str">
         <f>"25.03.2026"</f>
         <v>25.03.2026</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B3" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="13" t="s">
+      <c r="D3" s="13" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
-      <c r="A3" s="5"/>
-      <c r="B3" s="12"/>
-      <c r="C3" s="6"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="A4" s="5"/>
-      <c r="B4" s="6"/>
+      <c r="B4" s="12"/>
       <c r="C4" s="6"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.3">
@@ -572,14 +591,14 @@
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="5"/>
-      <c r="B10" s="7"/>
+      <c r="B10" s="6"/>
       <c r="C10" s="6"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="5"/>
-      <c r="B11" s="6"/>
+      <c r="B11" s="7"/>
       <c r="C11" s="6"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.3">
@@ -589,8 +608,8 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A13" s="5"/>
-      <c r="B13" s="5"/>
-      <c r="C13" s="5"/>
+      <c r="B13" s="6"/>
+      <c r="C13" s="6"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A14" s="5"/>
@@ -609,13 +628,13 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" s="5"/>
-      <c r="B17" s="8"/>
-      <c r="C17" s="8"/>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" s="5"/>
-      <c r="B18" s="5"/>
-      <c r="C18" s="5"/>
+      <c r="B18" s="8"/>
+      <c r="C18" s="8"/>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" s="5"/>
@@ -654,8 +673,8 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" s="5"/>
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
+      <c r="B26" s="5"/>
+      <c r="C26" s="5"/>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" s="5"/>
@@ -1223,9 +1242,9 @@
       <c r="C139" s="6"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="9"/>
-      <c r="B140" s="10"/>
-      <c r="C140" s="10"/>
+      <c r="A140" s="5"/>
+      <c r="B140" s="6"/>
+      <c r="C140" s="6"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="9"/>
@@ -5117,13 +5136,19 @@
       <c r="B918" s="10"/>
       <c r="C918" s="10"/>
     </row>
+    <row r="919" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A919" s="9"/>
+      <c r="B919" s="10"/>
+      <c r="C919" s="10"/>
+    </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{52F67EFF-01EC-4C1D-ACB7-B5A4E4927918}"/>
+    <hyperlink ref="D3" r:id="rId1" xr:uid="{52F67EFF-01EC-4C1D-ACB7-B5A4E4927918}"/>
+    <hyperlink ref="D2" r:id="rId2" xr:uid="{6AFCF0C3-4034-4D8B-8B24-5979CA798A9A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
-  <drawing r:id="rId2"/>
+  <drawing r:id="rId3"/>
 </worksheet>
 </file>
 

</xml_diff>